<commit_message>
Build 12 - Fixes for issues #8, #9, #10, #14
Signed-off-by: duncanamps <duncan@duncanamps.com>
</commit_message>
<xml_diff>
--- a/docs/opcode comparisons.xlsx
+++ b/docs/opcode comparisons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\asm80\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\xa80\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E848947-1701-4B7B-A6FF-D9A3D781CFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D56CF9-21B8-4605-972A-C6DC5222894E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="408" windowWidth="20004" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1296" yWindow="144" windowWidth="20004" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -845,7 +845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:A142"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Merge of main branch and preprocessor branch
Signed-off-by: duncanamps <duncan@duncanamps.com>
</commit_message>
<xml_diff>
--- a/docs/opcode comparisons.xlsx
+++ b/docs/opcode comparisons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\asm80\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\xa80\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E848947-1701-4B7B-A6FF-D9A3D781CFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D56CF9-21B8-4605-972A-C6DC5222894E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="408" windowWidth="20004" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1296" yWindow="144" windowWidth="20004" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -845,7 +845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:A142"/>
     </sheetView>
   </sheetViews>

</xml_diff>